<commit_message>
meds_tables_20240315 renamed to MEDS_Tables
</commit_message>
<xml_diff>
--- a/analysis/meds_tables_20240315.xlsx
+++ b/analysis/meds_tables_20240315.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.arboittedossantos\Shield Reply\UKHO - MEDS Replacement - Documents\MEDS DB\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{39F61ABB-3C1A-4B2A-8F36-B4F3678921B5}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="8_{5AE21C6D-DF2D-4912-BF4C-1DD1DB30D357}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A82BA9F-FBC3-441F-8899-A39896B91DFB}"/>
   <bookViews>
     <workbookView xWindow="-16005" yWindow="-21705" windowWidth="38625" windowHeight="21825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meds_tables!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">meds_tables!$A$1:$W$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$A$57</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="546">
   <si>
     <t>Table</t>
   </si>
@@ -1636,6 +1636,54 @@
   </si>
   <si>
     <t>10/11 2000</t>
+  </si>
+  <si>
+    <t>Confirm DATASET_INDEX is the key, and where it is used</t>
+  </si>
+  <si>
+    <t>How does it link to FIELD_LOOKUP?
+Confirm key (not found)
+It has TABLE_NAME</t>
+  </si>
+  <si>
+    <t>Confirm TYPE_INDEX is the key, and where is it used
+It has the column DATA_TYPE but it is null (JOB_LOOKUPS)</t>
+  </si>
+  <si>
+    <t>It probably wont be necessary since linked to current GIS
+There is a field named "Desciption"</t>
+  </si>
+  <si>
+    <t>Does the field DATA_TYPE_INDEX refer to JOB_LOOKUPS?
+It seems that the key has multiple columns
+There is one record with a data_type_index in field_lookup that is not in job_lookups (99)</t>
+  </si>
+  <si>
+    <t>Need a unique key, editor page is not working
+Confirm this is the master field table.
+Confirm key (not found)
+It has TABLE_NAME
+Does the field DATA_TYPE_INDEX refer to JOB_LOOKUPS?</t>
+  </si>
+  <si>
+    <t>It has TABLE_NAME
+It seems to contain two different kinds of data (definition &amp; display)
+Confirm key (not found), multiple keys
+Seems to have plenty of other foreign keys
+Many tables have columns as "data_require" and it is probably a boolean. Decide what to do with the modeland use of switches (implemented)</t>
+  </si>
+  <si>
+    <t>Unique index has multiple columns</t>
+  </si>
+  <si>
+    <t>Has nulls in many record names
+It probably wont be necessary since linked to current GIS</t>
+  </si>
+  <si>
+    <t>Has nulls in many record names</t>
+  </si>
+  <si>
+    <t>Essential</t>
   </si>
 </sst>
 </file>
@@ -2209,7 +2257,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2275,33 +2326,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86FB629C-F2E5-411E-AD4A-A055586C490B}" name="Table1" displayName="Table1" ref="A1:V194" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:V194" xr:uid="{926DB2D1-C889-4F81-AF44-99E61926DC0E}">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="10/11 2000"/>
-        <filter val="1010/1011"/>
-        <filter val="1020/1021"/>
-        <filter val="1030/1031"/>
-        <filter val="1040/1041"/>
-        <filter val="1050/1051"/>
-        <filter val="1060/1061"/>
-        <filter val="1070/1071"/>
-        <filter val="1080/1081"/>
-        <filter val="1090/1091"/>
-        <filter val="1100/1101"/>
-        <filter val="1110/1111"/>
-        <filter val="1120/1121"/>
-        <filter val="1130/1131"/>
-        <filter val="1140/1141"/>
-        <filter val="1150/1151"/>
-        <filter val="1160/1161"/>
-        <filter val="1170/1171"/>
-        <filter val="1180/1181"/>
-      </filters>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86FB629C-F2E5-411E-AD4A-A055586C490B}" name="Table1" displayName="Table1" ref="A1:W194" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:W194" xr:uid="{926DB2D1-C889-4F81-AF44-99E61926DC0E}">
+    <filterColumn colId="22">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="22">
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{61C27499-A67E-40B7-A5EA-168154BB80BC}" name="Table"/>
     <tableColumn id="2" xr3:uid="{44429CB3-B019-41CB-A78A-166C07FFEAD1}" name="Status"/>
     <tableColumn id="3" xr3:uid="{A8D54565-5DD9-422A-86EB-E9296F866224}" name="State/Use"/>
@@ -2313,16 +2346,17 @@
     <tableColumn id="9" xr3:uid="{2E1C974B-5E5C-464A-A28D-696BCE34F6CD}" name="Uploaded "/>
     <tableColumn id="10" xr3:uid="{266B087A-9D24-4171-8F11-705DADEC910B}" name="Upload Comments"/>
     <tableColumn id="11" xr3:uid="{FA5E8A8B-395C-466D-876B-C1B29EC2C0E5}" name="Action"/>
-    <tableColumn id="12" xr3:uid="{5680BC37-D731-4A82-8219-2D278BF018D7}" name="Type" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{F1E29237-FEC4-46DA-8853-96C12C596D65}" name="UI Type" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{8E330D8B-D10E-4961-9D55-8764B4BBC6E2}" name="UI Built" dataDxfId="6"/>
-    <tableColumn id="22" xr3:uid="{7E1AE159-50D1-46B9-A5B0-DB607D5B744D}" name="Pages" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{29F22248-BDD8-4CE0-851B-48DBBD8F9280}" name="Import" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{08C8FBD8-C984-4A7C-A4F1-93CA41D7503F}" name="Import Built" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{3EE11E24-F46E-4777-8793-796426D481E1}" name="Export" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{2C26C8C7-7DD0-49EB-BB8A-11E11250AAEB}" name="Export Built" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{5680BC37-D731-4A82-8219-2D278BF018D7}" name="Type" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{F1E29237-FEC4-46DA-8853-96C12C596D65}" name="UI Type" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{8E330D8B-D10E-4961-9D55-8764B4BBC6E2}" name="UI Built" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{7E1AE159-50D1-46B9-A5B0-DB607D5B744D}" name="Pages" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{29F22248-BDD8-4CE0-851B-48DBBD8F9280}" name="Import" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{08C8FBD8-C984-4A7C-A4F1-93CA41D7503F}" name="Import Built" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{3EE11E24-F46E-4777-8793-796426D481E1}" name="Export" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{2C26C8C7-7DD0-49EB-BB8A-11E11250AAEB}" name="Export Built" dataDxfId="2"/>
     <tableColumn id="19" xr3:uid="{AF6CE4E4-948A-484B-8CDC-F51993C8BA35}" name="Group"/>
-    <tableColumn id="20" xr3:uid="{C7CD444E-A891-43A1-B9A8-68A6DC5DF69E}" name="Confirmed" dataDxfId="0"/>
+    <tableColumn id="20" xr3:uid="{C7CD444E-A891-43A1-B9A8-68A6DC5DF69E}" name="Confirmed" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{422AA92E-BB41-4F05-A0DC-87786EC4D023}" name="Essential" dataDxfId="0"/>
     <tableColumn id="21" xr3:uid="{561E7942-2F06-4395-9B0F-EAB15703B160}" name="Data/UI Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2626,11 +2660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V194"/>
+  <dimension ref="A1:W194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S209" sqref="S209"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W88" sqref="W88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,11 +2690,12 @@
     <col min="19" max="19" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="58.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="58.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2724,11 +2759,14 @@
       <c r="U1" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2777,11 +2815,12 @@
       <c r="U2" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="7"/>
+      <c r="W2" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2827,9 +2866,10 @@
       <c r="U3" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V3"/>
-    </row>
-    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="7"/>
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2875,9 +2915,10 @@
       <c r="U4" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V4"/>
-    </row>
-    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="7"/>
+      <c r="W4"/>
+    </row>
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2923,13 +2964,14 @@
       <c r="U5" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V5"/>
-    </row>
-    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="V5" s="7"/>
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2965,13 +3007,14 @@
       <c r="U6" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V6"/>
-    </row>
-    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="V6" s="7"/>
+      <c r="W6"/>
+    </row>
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -3007,9 +3050,10 @@
       <c r="U7" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V7"/>
-    </row>
-    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V7" s="7"/>
+      <c r="W7"/>
+    </row>
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -3055,9 +3099,10 @@
       <c r="U8" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V8"/>
-    </row>
-    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="7"/>
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3103,13 +3148,14 @@
       <c r="U9" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V9"/>
-    </row>
-    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="V9" s="7"/>
+      <c r="W9"/>
+    </row>
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -3143,13 +3189,14 @@
       <c r="U10" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V10"/>
-    </row>
-    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="V10" s="7"/>
+      <c r="W10"/>
+    </row>
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -3183,13 +3230,14 @@
       <c r="U11" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V11"/>
-    </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="V11" s="7"/>
+      <c r="W11"/>
+    </row>
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -3223,13 +3271,14 @@
       <c r="U12" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V12"/>
-    </row>
-    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="V12" s="7"/>
+      <c r="W12"/>
+    </row>
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -3263,13 +3312,14 @@
       <c r="U13" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V13"/>
-    </row>
-    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="V13" s="7"/>
+      <c r="W13"/>
+    </row>
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -3303,13 +3353,14 @@
       <c r="U14" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V14"/>
-    </row>
-    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="V14" s="7"/>
+      <c r="W14"/>
+    </row>
+    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -3343,13 +3394,14 @@
       <c r="U15" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V15"/>
-    </row>
-    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="V15" s="7"/>
+      <c r="W15"/>
+    </row>
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -3392,13 +3444,14 @@
       <c r="U16" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V16"/>
-    </row>
-    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="V16" s="7"/>
+      <c r="W16"/>
+    </row>
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -3441,9 +3494,10 @@
       <c r="U17" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V17"/>
-    </row>
-    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V17" s="7"/>
+      <c r="W17"/>
+    </row>
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -3489,9 +3543,10 @@
       <c r="U18" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V18"/>
-    </row>
-    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="7"/>
+      <c r="W18"/>
+    </row>
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -3537,9 +3592,10 @@
       <c r="U19" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V19"/>
-    </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="7"/>
+      <c r="W19"/>
+    </row>
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -3582,9 +3638,10 @@
       <c r="U20" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V20"/>
-    </row>
-    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="7"/>
+      <c r="W20"/>
+    </row>
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -3627,9 +3684,10 @@
       <c r="U21" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V21"/>
-    </row>
-    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="7"/>
+      <c r="W21"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3642,11 +3700,12 @@
       <c r="U22" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V22" t="s">
+      <c r="V22" s="7"/>
+      <c r="W22" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="23" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3686,9 +3745,10 @@
       <c r="U23" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V23"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V23" s="7"/>
+      <c r="W23"/>
+    </row>
+    <row r="24" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -3737,9 +3797,12 @@
       <c r="U24" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V24"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V24" s="7"/>
+      <c r="W24" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3788,9 +3851,12 @@
       <c r="U25" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V25"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V25" s="7"/>
+      <c r="W25" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -3839,9 +3905,12 @@
       <c r="U26" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V26"/>
-    </row>
-    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V26" s="7"/>
+      <c r="W26" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -3887,9 +3956,10 @@
       <c r="U27" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V27"/>
-    </row>
-    <row r="28" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V27" s="7"/>
+      <c r="W27"/>
+    </row>
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -3935,13 +4005,14 @@
       <c r="U28" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V28"/>
-    </row>
-    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="V28" s="7"/>
+      <c r="W28"/>
+    </row>
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -3982,13 +4053,14 @@
       <c r="U29" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V29"/>
-    </row>
-    <row r="30" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="V29" s="7"/>
+      <c r="W29"/>
+    </row>
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -4029,13 +4101,14 @@
       <c r="U30" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V30"/>
-    </row>
-    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="V30" s="7"/>
+      <c r="W30"/>
+    </row>
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -4076,9 +4149,10 @@
       <c r="U31" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V31"/>
-    </row>
-    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V31" s="7"/>
+      <c r="W31"/>
+    </row>
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -4113,9 +4187,10 @@
       <c r="U32" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V32"/>
-    </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V32" s="7"/>
+      <c r="W32"/>
+    </row>
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -4158,9 +4233,10 @@
       <c r="U33" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V33"/>
-    </row>
-    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V33" s="7"/>
+      <c r="W33"/>
+    </row>
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -4203,9 +4279,10 @@
       <c r="U34" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V34"/>
-    </row>
-    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V34" s="7"/>
+      <c r="W34"/>
+    </row>
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -4248,9 +4325,10 @@
       <c r="U35" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V35"/>
-    </row>
-    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V35" s="7"/>
+      <c r="W35"/>
+    </row>
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -4293,9 +4371,10 @@
       <c r="U36" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V36"/>
-    </row>
-    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V36" s="7"/>
+      <c r="W36"/>
+    </row>
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -4338,9 +4417,10 @@
       <c r="U37" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V37"/>
-    </row>
-    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V37" s="7"/>
+      <c r="W37"/>
+    </row>
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -4383,9 +4463,10 @@
       <c r="U38" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V38"/>
-    </row>
-    <row r="39" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V38" s="7"/>
+      <c r="W38"/>
+    </row>
+    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -4428,9 +4509,10 @@
       <c r="U39" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V39"/>
-    </row>
-    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V39" s="7"/>
+      <c r="W39"/>
+    </row>
+    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -4473,9 +4555,10 @@
       <c r="U40" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V40"/>
-    </row>
-    <row r="41" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V40" s="7"/>
+      <c r="W40"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -4488,11 +4571,12 @@
       <c r="U41" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V41" t="s">
+      <c r="V41" s="7"/>
+      <c r="W41" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -4505,11 +4589,12 @@
       <c r="U42" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V42" t="s">
+      <c r="V42" s="7"/>
+      <c r="W42" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -4558,11 +4643,12 @@
       <c r="U43" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V43" t="s">
+      <c r="V43" s="7"/>
+      <c r="W43" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -4611,11 +4697,12 @@
       <c r="U44" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V44" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V44" s="7"/>
+      <c r="W44" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -4664,9 +4751,12 @@
       <c r="U45" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V45"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V45" s="7"/>
+      <c r="W45" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>116</v>
       </c>
@@ -4715,9 +4805,12 @@
       <c r="U46" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V46"/>
-    </row>
-    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V46" s="7"/>
+      <c r="W46" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -4760,9 +4853,10 @@
       <c r="U47" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V47"/>
-    </row>
-    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V47" s="7"/>
+      <c r="W47"/>
+    </row>
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -4805,9 +4899,10 @@
       <c r="U48" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V48"/>
-    </row>
-    <row r="49" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V48" s="7"/>
+      <c r="W48"/>
+    </row>
+    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>123</v>
       </c>
@@ -4850,9 +4945,10 @@
       <c r="U49" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V49"/>
-    </row>
-    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V49" s="7"/>
+      <c r="W49"/>
+    </row>
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>126</v>
       </c>
@@ -4895,9 +4991,10 @@
       <c r="U50" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V50"/>
-    </row>
-    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V50" s="7"/>
+      <c r="W50"/>
+    </row>
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>128</v>
       </c>
@@ -4940,9 +5037,10 @@
       <c r="U51" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V51"/>
-    </row>
-    <row r="52" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V51" s="7"/>
+      <c r="W51"/>
+    </row>
+    <row r="52" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -4991,9 +5089,10 @@
       <c r="U52" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V52"/>
-    </row>
-    <row r="53" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V52" s="7"/>
+      <c r="W52"/>
+    </row>
+    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>134</v>
       </c>
@@ -5042,9 +5141,10 @@
       <c r="U53" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V53"/>
-    </row>
-    <row r="54" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V53" s="7"/>
+      <c r="W53"/>
+    </row>
+    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>136</v>
       </c>
@@ -5093,9 +5193,10 @@
       <c r="U54" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V54"/>
-    </row>
-    <row r="55" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V54" s="7"/>
+      <c r="W54"/>
+    </row>
+    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>138</v>
       </c>
@@ -5138,9 +5239,10 @@
       <c r="U55" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V55"/>
-    </row>
-    <row r="56" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V55" s="7"/>
+      <c r="W55"/>
+    </row>
+    <row r="56" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>141</v>
       </c>
@@ -5183,9 +5285,10 @@
       <c r="U56" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V56"/>
-    </row>
-    <row r="57" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V56" s="7"/>
+      <c r="W56"/>
+    </row>
+    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -5228,9 +5331,10 @@
       <c r="U57" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V57"/>
-    </row>
-    <row r="58" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V57" s="7"/>
+      <c r="W57"/>
+    </row>
+    <row r="58" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>145</v>
       </c>
@@ -5273,9 +5377,10 @@
       <c r="U58" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V58"/>
-    </row>
-    <row r="59" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V58" s="7"/>
+      <c r="W58"/>
+    </row>
+    <row r="59" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>148</v>
       </c>
@@ -5318,9 +5423,10 @@
       <c r="U59" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V59"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V59" s="7"/>
+      <c r="W59"/>
+    </row>
+    <row r="60" spans="1:23" ht="120" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>150</v>
       </c>
@@ -5369,9 +5475,12 @@
       <c r="U60" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V60"/>
-    </row>
-    <row r="61" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V60" s="7"/>
+      <c r="W60" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>153</v>
       </c>
@@ -5414,9 +5523,10 @@
       <c r="U61" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V61"/>
-    </row>
-    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V61" s="7"/>
+      <c r="W61"/>
+    </row>
+    <row r="62" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>156</v>
       </c>
@@ -5459,9 +5569,10 @@
       <c r="U62" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V62"/>
-    </row>
-    <row r="63" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V62" s="7"/>
+      <c r="W62"/>
+    </row>
+    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>158</v>
       </c>
@@ -5504,9 +5615,10 @@
       <c r="U63" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V63"/>
-    </row>
-    <row r="64" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V63" s="7"/>
+      <c r="W63"/>
+    </row>
+    <row r="64" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>161</v>
       </c>
@@ -5549,9 +5661,10 @@
       <c r="U64" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V64"/>
-    </row>
-    <row r="65" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V64" s="7"/>
+      <c r="W64"/>
+    </row>
+    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>162</v>
       </c>
@@ -5597,9 +5710,10 @@
       <c r="U65" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V65"/>
-    </row>
-    <row r="66" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V65" s="7"/>
+      <c r="W65"/>
+    </row>
+    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>165</v>
       </c>
@@ -5645,9 +5759,10 @@
       <c r="U66" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V66"/>
-    </row>
-    <row r="67" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V66" s="7"/>
+      <c r="W66"/>
+    </row>
+    <row r="67" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>167</v>
       </c>
@@ -5681,9 +5796,10 @@
       <c r="U67" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V67"/>
-    </row>
-    <row r="68" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V67" s="7"/>
+      <c r="W67"/>
+    </row>
+    <row r="68" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>169</v>
       </c>
@@ -5726,9 +5842,10 @@
       <c r="U68" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V68"/>
-    </row>
-    <row r="69" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V68" s="7"/>
+      <c r="W68"/>
+    </row>
+    <row r="69" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>172</v>
       </c>
@@ -5771,9 +5888,10 @@
       <c r="U69" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V69"/>
-    </row>
-    <row r="70" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V69" s="7"/>
+      <c r="W69"/>
+    </row>
+    <row r="70" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>174</v>
       </c>
@@ -5816,9 +5934,10 @@
       <c r="U70" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V70"/>
-    </row>
-    <row r="71" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V70" s="7"/>
+      <c r="W70"/>
+    </row>
+    <row r="71" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>176</v>
       </c>
@@ -5853,9 +5972,10 @@
       <c r="U71" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V71"/>
-    </row>
-    <row r="72" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V71" s="7"/>
+      <c r="W71"/>
+    </row>
+    <row r="72" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>177</v>
       </c>
@@ -5889,9 +6009,10 @@
       <c r="U72" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V72"/>
-    </row>
-    <row r="73" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V72" s="7"/>
+      <c r="W72"/>
+    </row>
+    <row r="73" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>178</v>
       </c>
@@ -5925,9 +6046,10 @@
       <c r="U73" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V73"/>
-    </row>
-    <row r="74" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V73" s="7"/>
+      <c r="W73"/>
+    </row>
+    <row r="74" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>179</v>
       </c>
@@ -5970,9 +6092,10 @@
       <c r="U74" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V74"/>
-    </row>
-    <row r="75" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V74" s="7"/>
+      <c r="W74"/>
+    </row>
+    <row r="75" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -6015,9 +6138,10 @@
       <c r="U75" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V75"/>
-    </row>
-    <row r="76" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V75" s="7"/>
+      <c r="W75"/>
+    </row>
+    <row r="76" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>184</v>
       </c>
@@ -6060,9 +6184,10 @@
       <c r="U76" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V76"/>
-    </row>
-    <row r="77" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V76" s="7"/>
+      <c r="W76"/>
+    </row>
+    <row r="77" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>187</v>
       </c>
@@ -6105,9 +6230,10 @@
       <c r="U77" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V77"/>
-    </row>
-    <row r="78" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V77" s="7"/>
+      <c r="W77"/>
+    </row>
+    <row r="78" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>189</v>
       </c>
@@ -6150,9 +6276,10 @@
       <c r="U78" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V78"/>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V78" s="7"/>
+      <c r="W78"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>191</v>
       </c>
@@ -6201,9 +6328,12 @@
       <c r="U79" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V79"/>
-    </row>
-    <row r="80" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V79" s="7"/>
+      <c r="W79" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>194</v>
       </c>
@@ -6243,9 +6373,10 @@
       <c r="U80" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V80"/>
-    </row>
-    <row r="81" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V80" s="7"/>
+      <c r="W80"/>
+    </row>
+    <row r="81" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>197</v>
       </c>
@@ -6285,9 +6416,10 @@
       <c r="U81" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V81"/>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V81" s="7"/>
+      <c r="W81"/>
+    </row>
+    <row r="82" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -6321,9 +6453,10 @@
       <c r="U82" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V82"/>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V82" s="7"/>
+      <c r="W82"/>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>203</v>
       </c>
@@ -6372,11 +6505,12 @@
       <c r="U83" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V83" t="s">
+      <c r="V83" s="7"/>
+      <c r="W83" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>206</v>
       </c>
@@ -6425,9 +6559,10 @@
       <c r="U84" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V84"/>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V84" s="7"/>
+      <c r="W84"/>
+    </row>
+    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>208</v>
       </c>
@@ -6476,9 +6611,10 @@
       <c r="U85" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V85"/>
-    </row>
-    <row r="86" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V85" s="7"/>
+      <c r="W85"/>
+    </row>
+    <row r="86" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>210</v>
       </c>
@@ -6524,11 +6660,12 @@
       <c r="U86" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V86" t="s">
+      <c r="V86" s="7"/>
+      <c r="W86" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="87" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>215</v>
       </c>
@@ -6553,11 +6690,12 @@
       <c r="U87" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V87" t="s">
+      <c r="V87" s="7"/>
+      <c r="W87" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="88" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>219</v>
       </c>
@@ -6582,11 +6720,12 @@
       <c r="U88" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V88" t="s">
+      <c r="V88" s="7"/>
+      <c r="W88" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="89" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>223</v>
       </c>
@@ -6611,11 +6750,12 @@
       <c r="U89" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V89" t="s">
+      <c r="V89" s="7"/>
+      <c r="W89" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="90" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>227</v>
       </c>
@@ -6637,11 +6777,12 @@
       <c r="U90" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V90" t="s">
+      <c r="V90" s="7"/>
+      <c r="W90" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="91" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>230</v>
       </c>
@@ -6681,9 +6822,10 @@
       <c r="U91" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V91"/>
-    </row>
-    <row r="92" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V91" s="7"/>
+      <c r="W91"/>
+    </row>
+    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>233</v>
       </c>
@@ -6723,9 +6865,10 @@
       <c r="U92" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V92"/>
-    </row>
-    <row r="93" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V92" s="7"/>
+      <c r="W92"/>
+    </row>
+    <row r="93" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>236</v>
       </c>
@@ -6756,9 +6899,10 @@
       <c r="U93" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V93"/>
-    </row>
-    <row r="94" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V93" s="7"/>
+      <c r="W93"/>
+    </row>
+    <row r="94" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>237</v>
       </c>
@@ -6798,9 +6942,10 @@
       <c r="U94" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V94"/>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V94" s="7"/>
+      <c r="W94"/>
+    </row>
+    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>240</v>
       </c>
@@ -6849,9 +6994,10 @@
       <c r="U95" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V95"/>
-    </row>
-    <row r="96" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V95" s="7"/>
+      <c r="W95"/>
+    </row>
+    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>243</v>
       </c>
@@ -6879,9 +7025,10 @@
       <c r="U96" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V96"/>
-    </row>
-    <row r="97" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V96" s="7"/>
+      <c r="W96"/>
+    </row>
+    <row r="97" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>246</v>
       </c>
@@ -6927,9 +7074,10 @@
       <c r="U97" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V97"/>
-    </row>
-    <row r="98" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V97" s="7"/>
+      <c r="W97"/>
+    </row>
+    <row r="98" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>249</v>
       </c>
@@ -6975,9 +7123,10 @@
       <c r="U98" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V98"/>
-    </row>
-    <row r="99" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V98" s="7"/>
+      <c r="W98"/>
+    </row>
+    <row r="99" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>251</v>
       </c>
@@ -7023,9 +7172,10 @@
       <c r="U99" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V99"/>
-    </row>
-    <row r="100" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V99" s="7"/>
+      <c r="W99"/>
+    </row>
+    <row r="100" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>254</v>
       </c>
@@ -7071,9 +7221,10 @@
       <c r="U100" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V100"/>
-    </row>
-    <row r="101" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V100" s="7"/>
+      <c r="W100"/>
+    </row>
+    <row r="101" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>256</v>
       </c>
@@ -7119,9 +7270,10 @@
       <c r="U101" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V101"/>
-    </row>
-    <row r="102" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V101" s="7"/>
+      <c r="W101"/>
+    </row>
+    <row r="102" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>258</v>
       </c>
@@ -7167,9 +7319,10 @@
       <c r="U102" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V102"/>
-    </row>
-    <row r="103" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V102" s="7"/>
+      <c r="W102"/>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>260</v>
       </c>
@@ -7206,11 +7359,12 @@
       <c r="U103" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V103" t="s">
+      <c r="V103" s="7"/>
+      <c r="W103" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="104" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>263</v>
       </c>
@@ -7247,11 +7401,12 @@
       <c r="U104" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V104" t="s">
+      <c r="V104" s="7"/>
+      <c r="W104" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="105" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>264</v>
       </c>
@@ -7297,9 +7452,10 @@
       <c r="U105" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V105"/>
-    </row>
-    <row r="106" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V105" s="7"/>
+      <c r="W105"/>
+    </row>
+    <row r="106" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>267</v>
       </c>
@@ -7345,9 +7501,10 @@
       <c r="U106" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V106"/>
-    </row>
-    <row r="107" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V106" s="7"/>
+      <c r="W106"/>
+    </row>
+    <row r="107" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>269</v>
       </c>
@@ -7393,9 +7550,10 @@
       <c r="U107" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V107"/>
-    </row>
-    <row r="108" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V107" s="7"/>
+      <c r="W107"/>
+    </row>
+    <row r="108" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>272</v>
       </c>
@@ -7441,9 +7599,10 @@
       <c r="U108" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V108"/>
-    </row>
-    <row r="109" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V108" s="7"/>
+      <c r="W108"/>
+    </row>
+    <row r="109" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>274</v>
       </c>
@@ -7489,9 +7648,10 @@
       <c r="U109" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V109"/>
-    </row>
-    <row r="110" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V109" s="7"/>
+      <c r="W109"/>
+    </row>
+    <row r="110" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>277</v>
       </c>
@@ -7537,9 +7697,10 @@
       <c r="U110" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V110"/>
-    </row>
-    <row r="111" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V110" s="7"/>
+      <c r="W110"/>
+    </row>
+    <row r="111" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>279</v>
       </c>
@@ -7585,9 +7746,10 @@
       <c r="U111" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V111"/>
-    </row>
-    <row r="112" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V111" s="7"/>
+      <c r="W111"/>
+    </row>
+    <row r="112" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>282</v>
       </c>
@@ -7633,9 +7795,10 @@
       <c r="U112" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V112"/>
-    </row>
-    <row r="113" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V112" s="7"/>
+      <c r="W112"/>
+    </row>
+    <row r="113" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>284</v>
       </c>
@@ -7681,9 +7844,10 @@
       <c r="U113" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V113"/>
-    </row>
-    <row r="114" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V113" s="7"/>
+      <c r="W113"/>
+    </row>
+    <row r="114" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>287</v>
       </c>
@@ -7729,13 +7893,14 @@
       <c r="U114" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V114"/>
-    </row>
-    <row r="115" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
+      <c r="V114" s="7"/>
+      <c r="W114"/>
+    </row>
+    <row r="115" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>289</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" t="s">
         <v>16</v>
       </c>
       <c r="C115" s="4" t="s">
@@ -7778,13 +7943,14 @@
       <c r="U115" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V115"/>
-    </row>
-    <row r="116" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+      <c r="V115" s="7"/>
+      <c r="W115"/>
+    </row>
+    <row r="116" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>292</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" t="s">
         <v>16</v>
       </c>
       <c r="C116" s="4" t="s">
@@ -7827,9 +7993,10 @@
       <c r="U116" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V116"/>
-    </row>
-    <row r="117" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V116" s="7"/>
+      <c r="W116"/>
+    </row>
+    <row r="117" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>294</v>
       </c>
@@ -7875,9 +8042,10 @@
       <c r="U117" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V117"/>
-    </row>
-    <row r="118" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V117" s="7"/>
+      <c r="W117"/>
+    </row>
+    <row r="118" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>297</v>
       </c>
@@ -7923,9 +8091,10 @@
       <c r="U118" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V118"/>
-    </row>
-    <row r="119" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V118" s="7"/>
+      <c r="W118"/>
+    </row>
+    <row r="119" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>299</v>
       </c>
@@ -7956,9 +8125,10 @@
       <c r="U119" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V119"/>
-    </row>
-    <row r="120" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V119" s="7"/>
+      <c r="W119"/>
+    </row>
+    <row r="120" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>301</v>
       </c>
@@ -7989,9 +8159,10 @@
       <c r="U120" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V120"/>
-    </row>
-    <row r="121" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V120" s="7"/>
+      <c r="W120"/>
+    </row>
+    <row r="121" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>302</v>
       </c>
@@ -8034,9 +8205,10 @@
       <c r="U121" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V121"/>
-    </row>
-    <row r="122" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V121" s="7"/>
+      <c r="W121"/>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>304</v>
       </c>
@@ -8076,15 +8248,16 @@
       <c r="U122" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V122" t="s">
+      <c r="V122" s="7"/>
+      <c r="W122" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="123" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
+    <row r="123" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>306</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" t="s">
         <v>16</v>
       </c>
       <c r="C123" s="4" t="s">
@@ -8127,13 +8300,14 @@
       <c r="U123" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V123"/>
-    </row>
-    <row r="124" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
+      <c r="V123" s="7"/>
+      <c r="W123"/>
+    </row>
+    <row r="124" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>309</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" t="s">
         <v>16</v>
       </c>
       <c r="C124" s="4" t="s">
@@ -8176,9 +8350,10 @@
       <c r="U124" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V124"/>
-    </row>
-    <row r="125" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V124" s="7"/>
+      <c r="W124"/>
+    </row>
+    <row r="125" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>311</v>
       </c>
@@ -8227,9 +8402,10 @@
       <c r="U125" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V125"/>
-    </row>
-    <row r="126" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V125" s="7"/>
+      <c r="W125"/>
+    </row>
+    <row r="126" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>315</v>
       </c>
@@ -8278,9 +8454,10 @@
       <c r="U126" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V126"/>
-    </row>
-    <row r="127" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V126" s="7"/>
+      <c r="W126"/>
+    </row>
+    <row r="127" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>318</v>
       </c>
@@ -8329,9 +8506,10 @@
       <c r="U127" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V127"/>
-    </row>
-    <row r="128" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V127" s="7"/>
+      <c r="W127"/>
+    </row>
+    <row r="128" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>321</v>
       </c>
@@ -8380,9 +8558,10 @@
       <c r="U128" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V128"/>
-    </row>
-    <row r="129" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V128" s="7"/>
+      <c r="W128"/>
+    </row>
+    <row r="129" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>323</v>
       </c>
@@ -8431,9 +8610,10 @@
       <c r="U129" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V129"/>
-    </row>
-    <row r="130" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V129" s="7"/>
+      <c r="W129"/>
+    </row>
+    <row r="130" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>325</v>
       </c>
@@ -8482,9 +8662,10 @@
       <c r="U130" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V130"/>
-    </row>
-    <row r="131" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V130" s="7"/>
+      <c r="W130"/>
+    </row>
+    <row r="131" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>327</v>
       </c>
@@ -8533,9 +8714,10 @@
       <c r="U131" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V131"/>
-    </row>
-    <row r="132" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V131" s="7"/>
+      <c r="W131"/>
+    </row>
+    <row r="132" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>329</v>
       </c>
@@ -8584,9 +8766,10 @@
       <c r="U132" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V132"/>
-    </row>
-    <row r="133" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V132" s="7"/>
+      <c r="W132"/>
+    </row>
+    <row r="133" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>331</v>
       </c>
@@ -8635,9 +8818,10 @@
       <c r="U133" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V133"/>
-    </row>
-    <row r="134" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V133" s="7"/>
+      <c r="W133"/>
+    </row>
+    <row r="134" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>333</v>
       </c>
@@ -8671,9 +8855,10 @@
       <c r="U134" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V134"/>
-    </row>
-    <row r="135" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V134" s="7"/>
+      <c r="W134"/>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>335</v>
       </c>
@@ -8695,11 +8880,12 @@
       <c r="U135" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V135" t="s">
+      <c r="V135" s="7"/>
+      <c r="W135" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="136" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>338</v>
       </c>
@@ -8724,11 +8910,12 @@
       <c r="U136" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V136" t="s">
+      <c r="V136" s="7"/>
+      <c r="W136" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="137" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>342</v>
       </c>
@@ -8741,11 +8928,12 @@
       <c r="U137" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V137" t="s">
+      <c r="V137" s="7"/>
+      <c r="W137" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>344</v>
       </c>
@@ -8758,11 +8946,12 @@
       <c r="U138" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V138" t="s">
+      <c r="V138" s="7"/>
+      <c r="W138" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="139" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>345</v>
       </c>
@@ -8775,11 +8964,12 @@
       <c r="U139" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V139" t="s">
+      <c r="V139" s="7"/>
+      <c r="W139" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="140" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>346</v>
       </c>
@@ -8792,11 +8982,12 @@
       <c r="U140" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V140" t="s">
+      <c r="V140" s="7"/>
+      <c r="W140" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="141" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>347</v>
       </c>
@@ -8821,11 +9012,12 @@
       <c r="U141" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V141" t="s">
+      <c r="V141" s="7"/>
+      <c r="W141" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="142" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>351</v>
       </c>
@@ -8838,11 +9030,12 @@
       <c r="U142" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V142" t="s">
+      <c r="V142" s="7"/>
+      <c r="W142" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="143" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>352</v>
       </c>
@@ -8855,11 +9048,12 @@
       <c r="U143" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V143" t="s">
+      <c r="V143" s="7"/>
+      <c r="W143" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="144" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>353</v>
       </c>
@@ -8872,11 +9066,12 @@
       <c r="U144" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V144" t="s">
+      <c r="V144" s="7"/>
+      <c r="W144" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="145" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>354</v>
       </c>
@@ -8889,11 +9084,12 @@
       <c r="U145" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V145" t="s">
+      <c r="V145" s="7"/>
+      <c r="W145" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="146" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>355</v>
       </c>
@@ -8906,11 +9102,12 @@
       <c r="U146" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V146" t="s">
+      <c r="V146" s="7"/>
+      <c r="W146" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="147" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>356</v>
       </c>
@@ -8923,11 +9120,12 @@
       <c r="U147" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V147" t="s">
+      <c r="V147" s="7"/>
+      <c r="W147" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="148" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>357</v>
       </c>
@@ -8940,11 +9138,12 @@
       <c r="U148" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V148" t="s">
+      <c r="V148" s="7"/>
+      <c r="W148" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="149" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>358</v>
       </c>
@@ -8957,11 +9156,12 @@
       <c r="U149" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V149" t="s">
+      <c r="V149" s="7"/>
+      <c r="W149" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="150" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>359</v>
       </c>
@@ -8974,11 +9174,12 @@
       <c r="U150" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V150" t="s">
+      <c r="V150" s="7"/>
+      <c r="W150" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="151" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>360</v>
       </c>
@@ -8991,11 +9192,12 @@
       <c r="U151" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V151" t="s">
+      <c r="V151" s="7"/>
+      <c r="W151" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="152" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>361</v>
       </c>
@@ -9008,11 +9210,12 @@
       <c r="U152" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V152" t="s">
+      <c r="V152" s="7"/>
+      <c r="W152" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="153" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>362</v>
       </c>
@@ -9037,11 +9240,12 @@
       <c r="U153" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V153" t="s">
+      <c r="V153" s="7"/>
+      <c r="W153" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="154" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>365</v>
       </c>
@@ -9054,11 +9258,12 @@
       <c r="U154" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V154" t="s">
+      <c r="V154" s="7"/>
+      <c r="W154" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="155" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>366</v>
       </c>
@@ -9071,11 +9276,12 @@
       <c r="U155" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V155" t="s">
+      <c r="V155" s="7"/>
+      <c r="W155" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="156" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>367</v>
       </c>
@@ -9088,11 +9294,12 @@
       <c r="U156" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V156" t="s">
+      <c r="V156" s="7"/>
+      <c r="W156" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="157" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>368</v>
       </c>
@@ -9105,11 +9312,12 @@
       <c r="U157" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V157" t="s">
+      <c r="V157" s="7"/>
+      <c r="W157" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="158" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>369</v>
       </c>
@@ -9122,11 +9330,12 @@
       <c r="U158" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V158" t="s">
+      <c r="V158" s="7"/>
+      <c r="W158" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="159" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>370</v>
       </c>
@@ -9139,11 +9348,12 @@
       <c r="U159" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V159" t="s">
+      <c r="V159" s="7"/>
+      <c r="W159" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="160" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>371</v>
       </c>
@@ -9156,11 +9366,12 @@
       <c r="U160" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V160" t="s">
+      <c r="V160" s="7"/>
+      <c r="W160" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="161" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>372</v>
       </c>
@@ -9173,11 +9384,12 @@
       <c r="U161" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V161" t="s">
+      <c r="V161" s="7"/>
+      <c r="W161" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="162" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>373</v>
       </c>
@@ -9190,11 +9402,12 @@
       <c r="U162" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V162" t="s">
+      <c r="V162" s="7"/>
+      <c r="W162" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="163" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>374</v>
       </c>
@@ -9207,11 +9420,12 @@
       <c r="U163" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V163" t="s">
+      <c r="V163" s="7"/>
+      <c r="W163" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="164" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>375</v>
       </c>
@@ -9224,15 +9438,16 @@
       <c r="U164" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V164" t="s">
+      <c r="V164" s="7"/>
+      <c r="W164" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="165" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="4" t="s">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>376</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B165" t="s">
         <v>16</v>
       </c>
       <c r="C165" s="4" t="s">
@@ -9256,11 +9471,12 @@
       <c r="U165" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V165" t="s">
+      <c r="V165" s="7"/>
+      <c r="W165" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="166" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>380</v>
       </c>
@@ -9273,11 +9489,12 @@
       <c r="U166" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V166" t="s">
+      <c r="V166" s="7"/>
+      <c r="W166" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="167" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>381</v>
       </c>
@@ -9290,11 +9507,12 @@
       <c r="U167" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V167" t="s">
+      <c r="V167" s="7"/>
+      <c r="W167" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="168" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>382</v>
       </c>
@@ -9307,11 +9525,12 @@
       <c r="U168" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V168" t="s">
+      <c r="V168" s="7"/>
+      <c r="W168" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="169" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>383</v>
       </c>
@@ -9324,11 +9543,12 @@
       <c r="U169" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V169" t="s">
+      <c r="V169" s="7"/>
+      <c r="W169" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="170" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>384</v>
       </c>
@@ -9341,11 +9561,12 @@
       <c r="U170" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V170" t="s">
+      <c r="V170" s="7"/>
+      <c r="W170" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="171" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>385</v>
       </c>
@@ -9358,11 +9579,12 @@
       <c r="U171" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V171" t="s">
+      <c r="V171" s="7"/>
+      <c r="W171" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="172" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>386</v>
       </c>
@@ -9375,11 +9597,12 @@
       <c r="U172" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V172" t="s">
+      <c r="V172" s="7"/>
+      <c r="W172" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="173" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>387</v>
       </c>
@@ -9404,11 +9627,12 @@
       <c r="U173" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V173" t="s">
+      <c r="V173" s="7"/>
+      <c r="W173" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="174" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>391</v>
       </c>
@@ -9433,11 +9657,12 @@
       <c r="U174" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V174" t="s">
+      <c r="V174" s="7"/>
+      <c r="W174" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="175" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>395</v>
       </c>
@@ -9462,11 +9687,12 @@
       <c r="U175" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V175" t="s">
+      <c r="V175" s="7"/>
+      <c r="W175" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="176" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>399</v>
       </c>
@@ -9512,9 +9738,10 @@
       <c r="U176" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V176"/>
-    </row>
-    <row r="177" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V176" s="7"/>
+      <c r="W176"/>
+    </row>
+    <row r="177" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>402</v>
       </c>
@@ -9560,9 +9787,10 @@
       <c r="U177" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V177"/>
-    </row>
-    <row r="178" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V177" s="7"/>
+      <c r="W177"/>
+    </row>
+    <row r="178" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>404</v>
       </c>
@@ -9608,9 +9836,10 @@
       <c r="U178" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V178"/>
-    </row>
-    <row r="179" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V178" s="7"/>
+      <c r="W178"/>
+    </row>
+    <row r="179" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>407</v>
       </c>
@@ -9656,9 +9885,10 @@
       <c r="U179" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V179"/>
-    </row>
-    <row r="180" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V179" s="7"/>
+      <c r="W179"/>
+    </row>
+    <row r="180" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>409</v>
       </c>
@@ -9704,9 +9934,10 @@
       <c r="U180" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V180"/>
-    </row>
-    <row r="181" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V180" s="7"/>
+      <c r="W180"/>
+    </row>
+    <row r="181" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>412</v>
       </c>
@@ -9752,9 +9983,10 @@
       <c r="U181" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V181"/>
-    </row>
-    <row r="182" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V181" s="7"/>
+      <c r="W181"/>
+    </row>
+    <row r="182" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>414</v>
       </c>
@@ -9803,11 +10035,12 @@
       <c r="U182" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V182" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="183" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V182" s="7"/>
+      <c r="W182" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>417</v>
       </c>
@@ -9829,15 +10062,16 @@
       <c r="U183" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V183" t="s">
+      <c r="V183" s="7"/>
+      <c r="W183" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="184" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="4" t="s">
+    <row r="184" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>420</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" t="s">
         <v>16</v>
       </c>
       <c r="C184" s="4" t="s">
@@ -9880,13 +10114,14 @@
       <c r="U184" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V184"/>
-    </row>
-    <row r="185" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="4" t="s">
+      <c r="V184" s="7"/>
+      <c r="W184"/>
+    </row>
+    <row r="185" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>423</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B185" t="s">
         <v>16</v>
       </c>
       <c r="C185" s="4" t="s">
@@ -9926,9 +10161,10 @@
       <c r="U185" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V185"/>
-    </row>
-    <row r="186" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V185" s="7"/>
+      <c r="W185"/>
+    </row>
+    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>425</v>
       </c>
@@ -9977,11 +10213,12 @@
       <c r="U186" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V186" t="s">
+      <c r="V186" s="7"/>
+      <c r="W186" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="187" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>428</v>
       </c>
@@ -10012,11 +10249,12 @@
       <c r="U187" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V187" t="s">
+      <c r="V187" s="7"/>
+      <c r="W187" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="188" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>430</v>
       </c>
@@ -10032,11 +10270,12 @@
       <c r="U188" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V188" t="s">
+      <c r="V188" s="7"/>
+      <c r="W188" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="189" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>431</v>
       </c>
@@ -10058,11 +10297,12 @@
       <c r="U189" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V189" t="s">
+      <c r="V189" s="7"/>
+      <c r="W189" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="190" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>434</v>
       </c>
@@ -10105,9 +10345,10 @@
       <c r="U190" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V190"/>
-    </row>
-    <row r="191" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V190" s="7"/>
+      <c r="W190"/>
+    </row>
+    <row r="191" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>437</v>
       </c>
@@ -10147,9 +10388,10 @@
       <c r="U191" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V191"/>
-    </row>
-    <row r="192" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V191" s="7"/>
+      <c r="W191"/>
+    </row>
+    <row r="192" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>440</v>
       </c>
@@ -10189,9 +10431,10 @@
       <c r="U192" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V192"/>
-    </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V192" s="7"/>
+      <c r="W192"/>
+    </row>
+    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>442</v>
       </c>
@@ -10240,9 +10483,12 @@
       <c r="U193" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V193"/>
-    </row>
-    <row r="194" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V193" s="7"/>
+      <c r="W193" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="194" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>445</v>
       </c>
@@ -10291,8 +10537,9 @@
       <c r="U194" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="V194" t="s">
-        <v>484</v>
+      <c r="V194" s="7"/>
+      <c r="W194" s="2" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -10859,16 +11106,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{874513C8-4F6F-45FE-94D1-7393F18F743D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>